<commit_message>
mpv5 introduced a variable to represent device-type
</commit_message>
<xml_diff>
--- a/shCDP5.xlsx
+++ b/shCDP5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phe\Documents\tech\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D1914D-1F36-4585-9880-E268F1FB27C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FDE9B1-EA99-4E70-8A71-D71852F218D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19725" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="435" windowWidth="15345" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>g1/0/1</t>
   </si>
@@ -66,13 +66,25 @@
   </si>
   <si>
     <t>printer</t>
+  </si>
+  <si>
+    <t>wap</t>
+  </si>
+  <si>
+    <t>dvr</t>
+  </si>
+  <si>
+    <t>atm</t>
+  </si>
+  <si>
+    <t>floor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +215,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -906,84 +924,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>101</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>202</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>301</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>401</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>9</v>
       </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>401</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>